<commit_message>
add merged cells for fixtures
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -465,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:AH13"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -484,35 +484,55 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1"/>
+      <c r="G1"/>
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1"/>
+      <c r="J1"/>
+      <c r="K1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="L1"/>
+      <c r="M1"/>
+      <c r="N1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="O1"/>
+      <c r="P1"/>
+      <c r="Q1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="R1"/>
+      <c r="S1"/>
+      <c r="T1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="U1"/>
+      <c r="V1"/>
+      <c r="W1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
+      <c r="X1"/>
+      <c r="Y1"/>
+      <c r="Z1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA1"/>
+      <c r="AB1"/>
+      <c r="AC1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="AD1"/>
+      <c r="AE1"/>
+      <c r="AF1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="AG1"/>
+      <c r="AH1"/>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -526,7 +546,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -540,7 +560,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -554,7 +574,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -568,7 +588,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -582,7 +602,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -596,7 +616,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -610,7 +630,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -624,7 +644,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -638,7 +658,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -652,7 +672,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -666,7 +686,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -681,6 +701,18 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="Q1:S1"/>
+    <mergeCell ref="T1:V1"/>
+    <mergeCell ref="W1:Y1"/>
+    <mergeCell ref="Z1:AB1"/>
+    <mergeCell ref="AC1:AE1"/>
+    <mergeCell ref="AF1:AH1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>

</xml_diff>